<commit_message>
Mejora en los scripts de validación de formularios
</commit_message>
<xml_diff>
--- a/Sura/Emisión Motor - Varios vehiculos - Vehiculos.xlsx
+++ b/Sura/Emisión Motor - Varios vehiculos - Vehiculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ED7761-C02A-492B-A234-93115AF5A117}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2BE088-F0CF-4917-8952-01C97197E89C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F8708F9-7BC4-408F-93BD-D81A7ECC6DA1}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>